<commit_message>
chore: increase column width
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C3459-1D80-4276-AF16-E340F29A5DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1017BD8-2373-40E4-B5C0-54CDAEB71A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +521,7 @@
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Increase column width in excel template (#30)
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26C3459-1D80-4276-AF16-E340F29A5DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1017BD8-2373-40E4-B5C0-54CDAEB71A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +521,7 @@
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix: remove column for school name
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1017BD8-2373-40E4-B5C0-54CDAEB71A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46139EB-788D-45C5-A987-83837441BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -120,13 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -148,9 +146,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L1">
-    <sortCondition ref="A1:A2"/>
-  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
@@ -455,28 +450,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
@@ -506,10 +501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,12 +515,11 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -541,20 +535,17 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
School name is part of default values in Connectors.xlsx (#35)
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1017BD8-2373-40E4-B5C0-54CDAEB71A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46139EB-788D-45C5-A987-83837441BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -120,13 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -148,9 +146,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L1">
-    <sortCondition ref="A1:A2"/>
-  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
@@ -455,28 +450,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
@@ -506,10 +501,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,12 +515,11 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -541,20 +535,17 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add new values to PDF
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/school-module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46139EB-788D-45C5-A987-83837441BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1709F9-36D0-0446-8101-314EA306F4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="520" windowWidth="51220" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>connector-description</t>
+  </si>
+  <si>
+    <t>modules__school__playStoreLink</t>
+  </si>
+  <si>
+    <t>modules__school__appStoreLink</t>
   </si>
 </sst>
 </file>
@@ -127,8 +133,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,9 +150,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:N2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-port"/>
@@ -159,6 +165,8 @@
     <tableColumn id="10" xr3:uid="{C9357842-8DC4-4023-9A2E-A56E6E7245AA}" name="modules__school__schoolName"/>
     <tableColumn id="11" xr3:uid="{A40C4C2D-F55F-4A04-B6F8-52F87FA1FC8B}" name="modules__school__autoMailAfterOnboarding"/>
     <tableColumn id="12" xr3:uid="{DA2B806A-3C97-4465-A297-4FA4CAA89FA9}" name="modules__school__autoMailBeforeOffboarding"/>
+    <tableColumn id="13" xr3:uid="{7385C6FD-5B8F-1944-9FF6-84291A283000}" name="modules__school__playStoreLink"/>
+    <tableColumn id="14" xr3:uid="{4E46B1FA-1E3A-5B42-B9CB-31777F5F24AA}" name="modules__school__appStoreLink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,29 +435,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.33203125" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -486,8 +496,14 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>
@@ -501,25 +517,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -544,11 +562,18 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
App store links in pdfs (#40)
* feat: add store links

* feat: use store links

* feat: add new values to PDF
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tnotheis\src\enmeshed\connector-school-module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/school-module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46139EB-788D-45C5-A987-83837441BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1709F9-36D0-0446-8101-314EA306F4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="520" windowWidth="51220" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>connector-description</t>
+  </si>
+  <si>
+    <t>modules__school__playStoreLink</t>
+  </si>
+  <si>
+    <t>modules__school__appStoreLink</t>
   </si>
 </sst>
 </file>
@@ -127,8 +133,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,9 +150,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:N2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:N2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-port"/>
@@ -159,6 +165,8 @@
     <tableColumn id="10" xr3:uid="{C9357842-8DC4-4023-9A2E-A56E6E7245AA}" name="modules__school__schoolName"/>
     <tableColumn id="11" xr3:uid="{A40C4C2D-F55F-4A04-B6F8-52F87FA1FC8B}" name="modules__school__autoMailAfterOnboarding"/>
     <tableColumn id="12" xr3:uid="{DA2B806A-3C97-4465-A297-4FA4CAA89FA9}" name="modules__school__autoMailBeforeOffboarding"/>
+    <tableColumn id="13" xr3:uid="{7385C6FD-5B8F-1944-9FF6-84291A283000}" name="modules__school__playStoreLink"/>
+    <tableColumn id="14" xr3:uid="{4E46B1FA-1E3A-5B42-B9CB-31777F5F24AA}" name="modules__school__appStoreLink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -427,29 +435,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.33203125" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -486,8 +496,14 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>
@@ -501,25 +517,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -544,11 +562,18 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update the pdf
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/school-module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1709F9-36D0-0446-8101-314EA306F4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156F385B-72FE-2E46-AD14-58959F945295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="520" windowWidth="51220" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="520" windowWidth="51220" windowHeight="26920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>connector-description</t>
-  </si>
-  <si>
-    <t>modules__school__playStoreLink</t>
-  </si>
-  <si>
-    <t>modules__school__appStoreLink</t>
   </si>
 </sst>
 </file>
@@ -150,9 +144,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:N2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:N2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-port"/>
@@ -165,8 +159,6 @@
     <tableColumn id="10" xr3:uid="{C9357842-8DC4-4023-9A2E-A56E6E7245AA}" name="modules__school__schoolName"/>
     <tableColumn id="11" xr3:uid="{A40C4C2D-F55F-4A04-B6F8-52F87FA1FC8B}" name="modules__school__autoMailAfterOnboarding"/>
     <tableColumn id="12" xr3:uid="{DA2B806A-3C97-4465-A297-4FA4CAA89FA9}" name="modules__school__autoMailBeforeOffboarding"/>
-    <tableColumn id="13" xr3:uid="{7385C6FD-5B8F-1944-9FF6-84291A283000}" name="modules__school__playStoreLink"/>
-    <tableColumn id="14" xr3:uid="{4E46B1FA-1E3A-5B42-B9CB-31777F5F24AA}" name="modules__school__appStoreLink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,7 +451,7 @@
     <col min="14" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -496,14 +488,8 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>
@@ -519,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -562,12 +548,8 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>

</xml_diff>

<commit_message>
Make reference url format the default for the rendered QR code (#53)
* chore: update the config

* docs: update the pdf

* refactor: change config format

* feat: make reference url the default for the rendered qr code

* chore: update onboarding template

* chore: add down script
</commit_message>
<xml_diff>
--- a/Connectors.xlsx
+++ b/Connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkoenig/git/nmshd/school-module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1709F9-36D0-0446-8101-314EA306F4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156F385B-72FE-2E46-AD14-58959F945295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="520" windowWidth="51220" windowHeight="26920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="520" windowWidth="51220" windowHeight="26920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>backbone-base-url</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>connector-description</t>
-  </si>
-  <si>
-    <t>modules__school__playStoreLink</t>
-  </si>
-  <si>
-    <t>modules__school__appStoreLink</t>
   </si>
 </sst>
 </file>
@@ -150,9 +144,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:N2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:N2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}" name="Table1" displayName="Table1" ref="A1:L2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{3CFA046A-E24B-4843-8572-68A33A89E11B}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{33890D53-6763-4B54-8B8D-BCAC9A2EF139}" name="connector-id"/>
     <tableColumn id="2" xr3:uid="{272DDE2C-8254-4855-B433-2FFA394DB9A4}" name="connector-description"/>
     <tableColumn id="3" xr3:uid="{AC9F5FBE-4F34-404D-95B3-82665C59D054}" name="connector-port"/>
@@ -165,8 +159,6 @@
     <tableColumn id="10" xr3:uid="{C9357842-8DC4-4023-9A2E-A56E6E7245AA}" name="modules__school__schoolName"/>
     <tableColumn id="11" xr3:uid="{A40C4C2D-F55F-4A04-B6F8-52F87FA1FC8B}" name="modules__school__autoMailAfterOnboarding"/>
     <tableColumn id="12" xr3:uid="{DA2B806A-3C97-4465-A297-4FA4CAA89FA9}" name="modules__school__autoMailBeforeOffboarding"/>
-    <tableColumn id="13" xr3:uid="{7385C6FD-5B8F-1944-9FF6-84291A283000}" name="modules__school__playStoreLink"/>
-    <tableColumn id="14" xr3:uid="{4E46B1FA-1E3A-5B42-B9CB-31777F5F24AA}" name="modules__school__appStoreLink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,7 +451,7 @@
     <col min="14" max="14" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -496,14 +488,8 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
     </row>
   </sheetData>
@@ -519,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A291A44-47E4-425E-963E-799631E19E58}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -562,12 +548,8 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>

</xml_diff>